<commit_message>
branching logic has been changed
</commit_message>
<xml_diff>
--- a/scenarios/scenarios_Marxan_20190524.xlsx
+++ b/scenarios/scenarios_Marxan_20190524.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <fileSharing readOnlyRecommended="0" userName="pl"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId4"/>
@@ -18,10 +18,10 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1558842877" val="942" rev="123" revOS="4"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1558842877" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1558842877" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1558842877"/>
+      <pm:revision xmlns:pm="smNativeData" day="1566976962" val="962" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1566976962" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1566976962" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1566976962"/>
     </ext>
   </extLst>
 </workbook>
@@ -45,7 +45,7 @@
             <i val="0"/>
             <extLst>
               <ext uri="smNativeData">
-                <pm:charSpec xmlns:pm="smNativeData" id="1558842877">
+                <pm:charSpec xmlns:pm="smNativeData" id="1566976962">
                   <pm:latin face="Calibri" sz="220" weight="normal" i="0"/>
                   <pm:cs face="Calibri"/>
                   <pm:ea face="Calibri"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="360">
   <si>
     <t>#</t>
   </si>
@@ -1124,6 +1124,12 @@
   </si>
   <si>
     <t>Autumn</t>
+  </si>
+  <si>
+    <t>Distinctive</t>
+  </si>
+  <si>
+    <t>Representative</t>
   </si>
   <si>
     <t>PU_layers</t>
@@ -1160,7 +1166,7 @@
     <numFmt numFmtId="167" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="9" formatCode="0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="204"/>
@@ -1169,7 +1175,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1558842877" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1185,7 +1191,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1558842877" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -1201,7 +1207,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1558842877" fgClr="5983B0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" fgClr="5983B0" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1217,7 +1223,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1558842877" fgClr="7F7F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" fgClr="7F7F00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1233,7 +1239,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1558842877" fgClr="007F7F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" fgClr="007F7F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -1250,8 +1256,24 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1558842877" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
+            <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1566976962" ulstyle="none" kern="1">
+            <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
           </pm:charSpec>
@@ -1272,7 +1294,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1558842877" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1566976962" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1294,7 +1316,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1558842877"/>
+          <pm:border xmlns:pm="smNativeData" id="1566976962"/>
         </ext>
       </extLst>
     </border>
@@ -1313,7 +1335,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1558842877"/>
+          <pm:border xmlns:pm="smNativeData" id="1566976962"/>
         </ext>
       </extLst>
     </border>
@@ -1327,7 +1349,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2"/>
@@ -1345,6 +1367,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1358,10 +1381,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1558842877" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1566976962" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1558842877" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1566976962" count="1">
         <pm:color name="Color 24" rgb="5983B0"/>
       </pm:colors>
     </ext>
@@ -1589,7 +1612,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr>
+        <a:prstTxWarp prst="textNoShape">
+          <a:avLst/>
+        </a:prstTxWarp>
+        <a:noAutofit/>
+      </a:bodyPr>
+      <a:lstStyle>
+        <a:defPPr>
+          <a:defRPr/>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -1601,8 +1653,8 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -1757,7 +1809,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1558842877" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566976962" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1766,17 +1818,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1558842877" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566976962" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3592,7 +3644,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1558842877" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566976962" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3601,16 +3653,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1558842877" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566976962" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3624,11 +3676,11 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I200"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C131" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="J154" sqref="J154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -3639,7 +3691,7 @@
     <col min="1021" max="1025" width="11.517857" customWidth="1" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="9" t="str">
         <f>CF_list!A1</f>
         <v>CF_code</v>
@@ -3669,8 +3721,14 @@
       <c r="I1" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="J1" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="9">
         <f>CF_list!A2</f>
         <v>3002</v>
@@ -3685,8 +3743,11 @@
       <c r="D2" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="9">
         <f>CF_list!A3</f>
         <v>3004</v>
@@ -3701,8 +3762,11 @@
       <c r="D3" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="9">
         <f>CF_list!A4</f>
         <v>3006</v>
@@ -3717,8 +3781,11 @@
       <c r="D4" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="9">
         <f>CF_list!A5</f>
         <v>3008</v>
@@ -3733,8 +3800,11 @@
       <c r="D5" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="9">
         <f>CF_list!A6</f>
         <v>3010</v>
@@ -3749,8 +3819,11 @@
       <c r="D6" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="9">
         <f>CF_list!A7</f>
         <v>3012</v>
@@ -3765,8 +3838,11 @@
       <c r="D7" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="9">
         <f>CF_list!A8</f>
         <v>3014</v>
@@ -3781,8 +3857,11 @@
       <c r="D8" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="9">
         <f>CF_list!A9</f>
         <v>3016</v>
@@ -3797,8 +3876,11 @@
       <c r="D9" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="9">
         <f>CF_list!A10</f>
         <v>3018</v>
@@ -3813,8 +3895,11 @@
       <c r="D10" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="9">
         <f>CF_list!A11</f>
         <v>3020</v>
@@ -3829,8 +3914,11 @@
       <c r="D11" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="9">
         <f>CF_list!A12</f>
         <v>3022</v>
@@ -3845,8 +3933,11 @@
       <c r="D12" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="9">
         <f>CF_list!A13</f>
         <v>3024</v>
@@ -3861,8 +3952,11 @@
       <c r="D13" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="9">
         <f>CF_list!A14</f>
         <v>3026</v>
@@ -3877,8 +3971,11 @@
       <c r="D14" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="9">
         <f>CF_list!A15</f>
         <v>3028</v>
@@ -3893,8 +3990,11 @@
       <c r="D15" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="9">
         <f>CF_list!A16</f>
         <v>3030</v>
@@ -3909,8 +4009,11 @@
       <c r="D16" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="9">
         <f>CF_list!A17</f>
         <v>3032</v>
@@ -3925,8 +4028,11 @@
       <c r="D17" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="9">
         <f>CF_list!A18</f>
         <v>3033</v>
@@ -3941,8 +4047,14 @@
       <c r="D18" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="9">
         <f>CF_list!A19</f>
         <v>3034</v>
@@ -3957,8 +4069,14 @@
       <c r="D19" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="J19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="9">
         <f>CF_list!A20</f>
         <v>3035</v>
@@ -3973,8 +4091,14 @@
       <c r="D20" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="J20" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="9">
         <f>CF_list!A21</f>
         <v>3036</v>
@@ -3989,8 +4113,14 @@
       <c r="D21" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="9">
         <f>CF_list!A22</f>
         <v>3037</v>
@@ -4005,8 +4135,14 @@
       <c r="D22" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="J22" t="n">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="9">
         <f>CF_list!A23</f>
         <v>3038</v>
@@ -4021,8 +4157,14 @@
       <c r="D23" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="9">
         <f>CF_list!A24</f>
         <v>3041</v>
@@ -4037,8 +4179,14 @@
       <c r="D24" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="9">
         <f>CF_list!A25</f>
         <v>3043</v>
@@ -4053,8 +4201,14 @@
       <c r="D25" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="J25" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="9">
         <f>CF_list!A26</f>
         <v>3044</v>
@@ -4069,8 +4223,14 @@
       <c r="D26" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="9">
         <f>CF_list!A27</f>
         <v>3045</v>
@@ -4085,8 +4245,14 @@
       <c r="D27" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="J27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="9">
         <f>CF_list!A28</f>
         <v>3046</v>
@@ -4101,8 +4267,14 @@
       <c r="D28" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="9">
         <f>CF_list!A29</f>
         <v>3048</v>
@@ -4117,8 +4289,14 @@
       <c r="D29" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="9">
         <f>CF_list!A30</f>
         <v>3050</v>
@@ -4133,8 +4311,14 @@
       <c r="D30" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="J30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="9">
         <f>CF_list!A31</f>
         <v>3052</v>
@@ -4149,8 +4333,14 @@
       <c r="D31" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="9">
         <f>CF_list!A32</f>
         <v>3054</v>
@@ -4165,8 +4355,14 @@
       <c r="D32" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="9">
         <f>CF_list!A33</f>
         <v>3056</v>
@@ -4181,8 +4377,14 @@
       <c r="D33" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="9">
         <f>CF_list!A34</f>
         <v>3058</v>
@@ -4197,8 +4399,14 @@
       <c r="D34" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="9">
         <f>CF_list!A35</f>
         <v>3060</v>
@@ -4213,8 +4421,14 @@
       <c r="D35" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="9">
         <f>CF_list!A36</f>
         <v>3062</v>
@@ -4229,8 +4443,14 @@
       <c r="D36" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="9">
         <f>CF_list!A37</f>
         <v>3064</v>
@@ -4245,8 +4465,14 @@
       <c r="D37" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="J37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="9">
         <f>CF_list!A38</f>
         <v>3066</v>
@@ -4261,8 +4487,14 @@
       <c r="D38" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="9">
         <f>CF_list!A39</f>
         <v>3068</v>
@@ -4277,8 +4509,14 @@
       <c r="D39" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="9">
         <f>CF_list!A40</f>
         <v>3070</v>
@@ -4293,8 +4531,14 @@
       <c r="D40" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="J40" t="n">
+        <v>1</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="9">
         <f>CF_list!A41</f>
         <v>3072</v>
@@ -4309,8 +4553,14 @@
       <c r="D41" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="J41" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="9">
         <f>CF_list!A42</f>
         <v>3074</v>
@@ -4325,8 +4575,14 @@
       <c r="D42" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="J42" t="n">
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="9">
         <f>CF_list!A43</f>
         <v>3076</v>
@@ -4341,8 +4597,14 @@
       <c r="D43" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="J43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="9">
         <f>CF_list!A44</f>
         <v>3078</v>
@@ -4357,8 +4619,14 @@
       <c r="D44" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="J44" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="9">
         <f>CF_list!A45</f>
         <v>3080</v>
@@ -4373,8 +4641,14 @@
       <c r="D45" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="J45" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="9">
         <f>CF_list!A46</f>
         <v>3082</v>
@@ -4389,8 +4663,14 @@
       <c r="D46" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="J46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="9">
         <f>CF_list!A47</f>
         <v>3084</v>
@@ -4403,8 +4683,14 @@
         <v>1</v>
       </c>
       <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="J47" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="9">
         <f>CF_list!A48</f>
         <v>3085</v>
@@ -4419,8 +4705,14 @@
       <c r="D48" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="J48" t="n">
+        <v>1</v>
+      </c>
+      <c r="K48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="9">
         <f>CF_list!A49</f>
         <v>3086</v>
@@ -4435,8 +4727,14 @@
       <c r="D49" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="J49" t="n">
+        <v>1</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="9">
         <f>CF_list!A50</f>
         <v>3087</v>
@@ -4451,8 +4749,14 @@
       <c r="D50" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="J50" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="9">
         <f>CF_list!A51</f>
         <v>3088</v>
@@ -4467,8 +4771,14 @@
       <c r="D51" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="J51" t="n">
+        <v>1</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="9">
         <f>CF_list!A52</f>
         <v>3089</v>
@@ -4483,8 +4793,14 @@
       <c r="D52" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="J52" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="9">
         <f>CF_list!A53</f>
         <v>3090</v>
@@ -4499,8 +4815,14 @@
       <c r="D53" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="J53" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="9">
         <f>CF_list!A54</f>
         <v>3091</v>
@@ -4515,8 +4837,14 @@
       <c r="D54" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="J54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="9">
         <f>CF_list!A55</f>
         <v>3092</v>
@@ -4531,8 +4859,14 @@
       <c r="D55" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="J55" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="9">
         <f>CF_list!A56</f>
         <v>3093</v>
@@ -4547,8 +4881,14 @@
       <c r="D56" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="J56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="9">
         <f>CF_list!A57</f>
         <v>3094</v>
@@ -4563,8 +4903,14 @@
       <c r="D57" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="9">
         <f>CF_list!A58</f>
         <v>3095</v>
@@ -4579,8 +4925,14 @@
       <c r="D58" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="9">
         <f>CF_list!A59</f>
         <v>3096</v>
@@ -4595,8 +4947,14 @@
       <c r="D59" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="J59" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="9">
         <f>CF_list!A60</f>
         <v>3097</v>
@@ -4611,8 +4969,14 @@
       <c r="D60" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="J60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="9">
         <f>CF_list!A61</f>
         <v>3098</v>
@@ -4627,8 +4991,14 @@
       <c r="D61" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="J61" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="9">
         <f>CF_list!A62</f>
         <v>3099</v>
@@ -4643,8 +5013,14 @@
       <c r="D62" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="J62" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="9">
         <f>CF_list!A63</f>
         <v>3100</v>
@@ -4659,8 +5035,14 @@
       <c r="D63" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="J63" t="n">
+        <v>1</v>
+      </c>
+      <c r="K63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="9">
         <f>CF_list!A64</f>
         <v>3101</v>
@@ -4675,8 +5057,14 @@
       <c r="D64" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="J64" t="n">
+        <v>1</v>
+      </c>
+      <c r="K64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="9">
         <f>CF_list!A65</f>
         <v>3102</v>
@@ -4691,8 +5079,14 @@
       <c r="D65" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="J65" t="n">
+        <v>1</v>
+      </c>
+      <c r="K65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="9">
         <f>CF_list!A66</f>
         <v>3103</v>
@@ -4707,8 +5101,14 @@
       <c r="D66" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="J66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="9">
         <f>CF_list!A67</f>
         <v>9201</v>
@@ -4729,8 +5129,11 @@
       <c r="F67" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="J67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="9">
         <f>CF_list!A68</f>
         <v>9202</v>
@@ -4751,8 +5154,11 @@
       <c r="F68" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="J68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="9">
         <f>CF_list!A69</f>
         <v>9203</v>
@@ -4773,8 +5179,11 @@
       <c r="F69" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="J69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="9">
         <f>CF_list!A70</f>
         <v>9204</v>
@@ -4795,8 +5204,11 @@
       <c r="F70" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="J70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="9">
         <f>CF_list!A71</f>
         <v>9205</v>
@@ -4817,8 +5229,11 @@
       <c r="F71" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="J71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="9">
         <f>CF_list!A72</f>
         <v>9206</v>
@@ -4839,8 +5254,11 @@
       <c r="F72" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="J72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="9">
         <f>CF_list!A73</f>
         <v>9207</v>
@@ -4861,8 +5279,11 @@
       <c r="F73" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="J73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="9">
         <f>CF_list!A74</f>
         <v>9208</v>
@@ -4883,8 +5304,11 @@
       <c r="F74" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="J74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="9">
         <f>CF_list!A75</f>
         <v>9209</v>
@@ -4905,8 +5329,11 @@
       <c r="F75" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="J75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="9">
         <f>CF_list!A76</f>
         <v>9210</v>
@@ -4927,8 +5354,11 @@
       <c r="F76" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="J76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" s="9">
         <f>CF_list!A77</f>
         <v>9211</v>
@@ -4949,8 +5379,11 @@
       <c r="F77" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="J77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" s="9">
         <f>CF_list!A78</f>
         <v>9212</v>
@@ -4971,8 +5404,11 @@
       <c r="F78" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="J78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" s="9">
         <f>CF_list!A79</f>
         <v>9213</v>
@@ -4993,8 +5429,11 @@
       <c r="F79" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="J79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="9">
         <f>CF_list!A80</f>
         <v>9214</v>
@@ -5015,8 +5454,11 @@
       <c r="F80" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="J80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="9">
         <f>CF_list!A81</f>
         <v>9215</v>
@@ -5037,8 +5479,11 @@
       <c r="F81" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="J81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="9">
         <f>CF_list!A82</f>
         <v>9216</v>
@@ -5059,8 +5504,11 @@
       <c r="F82" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="J82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="9">
         <f>CF_list!A83</f>
         <v>9217</v>
@@ -5081,8 +5529,11 @@
       <c r="F83" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="J83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="9">
         <f>CF_list!A84</f>
         <v>9218</v>
@@ -5103,8 +5554,11 @@
       <c r="F84" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="J84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="9">
         <f>CF_list!A85</f>
         <v>9219</v>
@@ -5125,8 +5579,11 @@
       <c r="F85" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="J85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="9">
         <f>CF_list!A86</f>
         <v>9299</v>
@@ -5140,8 +5597,11 @@
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="J86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="9">
         <f>CF_list!A87</f>
         <v>9301</v>
@@ -5162,8 +5622,11 @@
       <c r="G87" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="J87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="9">
         <f>CF_list!A88</f>
         <v>9302</v>
@@ -5184,8 +5647,11 @@
       <c r="G88" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="J88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="9">
         <f>CF_list!A89</f>
         <v>9303</v>
@@ -5206,8 +5672,11 @@
       <c r="G89" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="J89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="9">
         <f>CF_list!A90</f>
         <v>9304</v>
@@ -5228,8 +5697,11 @@
       <c r="G90" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="J90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="9">
         <f>CF_list!A91</f>
         <v>9305</v>
@@ -5250,8 +5722,11 @@
       <c r="G91" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="J91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="9">
         <f>CF_list!A92</f>
         <v>9306</v>
@@ -5272,8 +5747,11 @@
       <c r="G92" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="J92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="9">
         <f>CF_list!A93</f>
         <v>9307</v>
@@ -5294,8 +5772,11 @@
       <c r="G93" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="J93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="9">
         <f>CF_list!A94</f>
         <v>9308</v>
@@ -5316,8 +5797,11 @@
       <c r="G94" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="J94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="9">
         <f>CF_list!A95</f>
         <v>9309</v>
@@ -5338,8 +5822,11 @@
       <c r="G95" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="J95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="9">
         <f>CF_list!A96</f>
         <v>9310</v>
@@ -5360,8 +5847,11 @@
       <c r="G96" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="J96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="9">
         <f>CF_list!A97</f>
         <v>9311</v>
@@ -5382,8 +5872,11 @@
       <c r="G97" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="J97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="9">
         <f>CF_list!A98</f>
         <v>9312</v>
@@ -5404,8 +5897,11 @@
       <c r="G98" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="J98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="9">
         <f>CF_list!A99</f>
         <v>9313</v>
@@ -5426,8 +5922,11 @@
       <c r="G99" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="J99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="9">
         <f>CF_list!A100</f>
         <v>9314</v>
@@ -5448,8 +5947,11 @@
       <c r="G100" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="J100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="9">
         <f>CF_list!A101</f>
         <v>9315</v>
@@ -5470,8 +5972,11 @@
       <c r="G101" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:7">
+      <c r="J101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="9">
         <f>CF_list!A102</f>
         <v>9316</v>
@@ -5492,8 +5997,11 @@
       <c r="G102" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="J102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="9">
         <f>CF_list!A103</f>
         <v>9317</v>
@@ -5514,8 +6022,11 @@
       <c r="G103" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="J103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="9">
         <f>CF_list!A104</f>
         <v>9318</v>
@@ -5536,8 +6047,11 @@
       <c r="G104" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="J104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="9">
         <f>CF_list!A105</f>
         <v>9319</v>
@@ -5558,8 +6072,11 @@
       <c r="G105" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="J105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="9">
         <f>CF_list!A106</f>
         <v>9399</v>
@@ -5573,8 +6090,11 @@
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="8"/>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="J106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" s="9">
         <f>CF_list!A107</f>
         <v>9401</v>
@@ -5595,8 +6115,11 @@
       <c r="H107" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="J107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" s="9">
         <f>CF_list!A108</f>
         <v>9402</v>
@@ -5617,8 +6140,11 @@
       <c r="H108" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="J108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" s="9">
         <f>CF_list!A109</f>
         <v>9403</v>
@@ -5639,8 +6165,11 @@
       <c r="H109" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="J109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" s="9">
         <f>CF_list!A110</f>
         <v>9404</v>
@@ -5661,8 +6190,11 @@
       <c r="H110" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="J110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" s="9">
         <f>CF_list!A111</f>
         <v>9406</v>
@@ -5683,8 +6215,11 @@
       <c r="H111" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="J111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" s="9">
         <f>CF_list!A112</f>
         <v>9407</v>
@@ -5705,8 +6240,11 @@
       <c r="H112" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="9">
         <f>CF_list!A113</f>
         <v>9408</v>
@@ -5727,8 +6265,11 @@
       <c r="H113" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="9">
         <f>CF_list!A114</f>
         <v>9409</v>
@@ -5749,8 +6290,11 @@
       <c r="H114" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="9">
         <f>CF_list!A115</f>
         <v>9410</v>
@@ -5771,8 +6315,11 @@
       <c r="H115" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" s="9">
         <f>CF_list!A116</f>
         <v>9411</v>
@@ -5793,8 +6340,11 @@
       <c r="H116" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="9">
         <f>CF_list!A117</f>
         <v>9412</v>
@@ -5815,8 +6365,11 @@
       <c r="H117" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="J117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" s="9">
         <f>CF_list!A118</f>
         <v>9413</v>
@@ -5837,8 +6390,11 @@
       <c r="H118" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:9">
+      <c r="J118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="9">
         <f>CF_list!A119</f>
         <v>9414</v>
@@ -5859,8 +6415,11 @@
       <c r="H119" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="J119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="9">
         <f>CF_list!A120</f>
         <v>9415</v>
@@ -5881,8 +6440,11 @@
       <c r="H120" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="J120" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="9">
         <f>CF_list!A121</f>
         <v>9416</v>
@@ -5903,8 +6465,11 @@
       <c r="H121" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="J121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="9">
         <f>CF_list!A122</f>
         <v>9418</v>
@@ -5925,8 +6490,11 @@
       <c r="H122" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="J122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="9">
         <f>CF_list!A123</f>
         <v>9499</v>
@@ -5940,8 +6508,11 @@
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="J123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="9">
         <f>CF_list!A124</f>
         <v>9501</v>
@@ -5962,8 +6533,11 @@
       <c r="I124" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="J124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="9">
         <f>CF_list!A125</f>
         <v>9502</v>
@@ -5984,8 +6558,11 @@
       <c r="I125" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="J125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" s="9">
         <f>CF_list!A126</f>
         <v>9503</v>
@@ -6006,8 +6583,11 @@
       <c r="I126" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="J126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="9">
         <f>CF_list!A127</f>
         <v>9504</v>
@@ -6028,8 +6608,11 @@
       <c r="I127" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="J127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" s="9">
         <f>CF_list!A128</f>
         <v>9505</v>
@@ -6050,8 +6633,11 @@
       <c r="I128" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" s="9">
         <f>CF_list!A129</f>
         <v>9506</v>
@@ -6072,8 +6658,11 @@
       <c r="I129" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:9">
+      <c r="J129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130" s="9">
         <f>CF_list!A130</f>
         <v>9507</v>
@@ -6094,8 +6683,11 @@
       <c r="I130" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:9">
+      <c r="J130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131" s="9">
         <f>CF_list!A131</f>
         <v>9508</v>
@@ -6116,8 +6708,11 @@
       <c r="I131" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:9">
+      <c r="J131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132" s="9">
         <f>CF_list!A132</f>
         <v>9509</v>
@@ -6138,8 +6733,11 @@
       <c r="I132" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:9">
+      <c r="J132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133" s="9">
         <f>CF_list!A133</f>
         <v>9510</v>
@@ -6160,8 +6758,11 @@
       <c r="I133" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:9">
+      <c r="J133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134" s="9">
         <f>CF_list!A134</f>
         <v>9511</v>
@@ -6182,8 +6783,11 @@
       <c r="I134" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:9">
+      <c r="J134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135" s="9">
         <f>CF_list!A135</f>
         <v>9512</v>
@@ -6204,8 +6808,11 @@
       <c r="I135" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:9">
+      <c r="J135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136" s="9">
         <f>CF_list!A136</f>
         <v>9513</v>
@@ -6226,8 +6833,11 @@
       <c r="I136" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:9">
+      <c r="J136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137" s="9">
         <f>CF_list!A137</f>
         <v>9514</v>
@@ -6248,8 +6858,11 @@
       <c r="I137" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="J137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138" s="9">
         <f>CF_list!A138</f>
         <v>9515</v>
@@ -6270,8 +6883,11 @@
       <c r="I138" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="J138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139" s="9">
         <f>CF_list!A139</f>
         <v>9516</v>
@@ -6292,8 +6908,11 @@
       <c r="I139" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:9">
+      <c r="J139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140" s="9">
         <f>CF_list!A140</f>
         <v>9517</v>
@@ -6314,8 +6933,11 @@
       <c r="I140" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:9">
+      <c r="J140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141" s="9">
         <f>CF_list!A141</f>
         <v>9518</v>
@@ -6336,8 +6958,11 @@
       <c r="I141" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:9">
+      <c r="J141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142" s="9">
         <f>CF_list!A142</f>
         <v>9519</v>
@@ -6358,8 +6983,11 @@
       <c r="I142" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="J142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143" s="9">
         <f>CF_list!A143</f>
         <v>9599</v>
@@ -6373,8 +7001,11 @@
       </c>
       <c r="D143" s="8"/>
       <c r="E143" s="8"/>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="J143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144" s="9">
         <f>CF_list!A144</f>
         <v>3203</v>
@@ -6389,8 +7020,11 @@
       <c r="D144" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="J144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145" s="9">
         <f>CF_list!A145</f>
         <v>3205</v>
@@ -6405,8 +7039,11 @@
       <c r="D145" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="J145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146" s="9">
         <f>CF_list!A146</f>
         <v>3206</v>
@@ -6421,8 +7058,11 @@
       <c r="D146" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="J146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147" s="9">
         <f>CF_list!A147</f>
         <v>3207</v>
@@ -6437,8 +7077,11 @@
       <c r="D147" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="J147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148" s="9">
         <f>CF_list!A148</f>
         <v>3208</v>
@@ -6453,8 +7096,11 @@
       <c r="D148" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="J148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149" s="9">
         <f>CF_list!A149</f>
         <v>3212</v>
@@ -6469,8 +7115,11 @@
       <c r="D149" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="J149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150" s="9">
         <f>CF_list!A150</f>
         <v>3213</v>
@@ -6485,8 +7134,11 @@
       <c r="D150" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:4">
+      <c r="J150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151" s="9">
         <f>CF_list!A151</f>
         <v>3214</v>
@@ -6501,8 +7153,11 @@
       <c r="D151" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="J151" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152" s="9">
         <f>CF_list!A152</f>
         <v>3215</v>
@@ -6517,8 +7172,11 @@
       <c r="D152" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:4">
+      <c r="J152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153" s="9">
         <f>CF_list!A153</f>
         <v>3216</v>
@@ -6533,8 +7191,11 @@
       <c r="D153" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:4">
+      <c r="J153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154" s="9">
         <f>CF_list!A154</f>
         <v>3217</v>
@@ -6549,8 +7210,11 @@
       <c r="D154" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:4">
+      <c r="J154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155" s="9">
         <f>CF_list!A155</f>
         <v>3218</v>
@@ -6565,8 +7229,11 @@
       <c r="D155" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
+      <c r="J155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156" s="9">
         <f>CF_list!A156</f>
         <v>3299</v>
@@ -6579,8 +7246,11 @@
         <v>1</v>
       </c>
       <c r="D156" s="8"/>
-    </row>
-    <row r="157" spans="1:9">
+      <c r="J156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
       <c r="A157" s="9">
         <f>CF_list!A157</f>
         <v>3301</v>
@@ -6605,8 +7275,11 @@
       <c r="I157" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:9">
+      <c r="K157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11">
       <c r="A158" s="9">
         <f>CF_list!A158</f>
         <v>3302</v>
@@ -6631,8 +7304,14 @@
       <c r="I158" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:9">
+      <c r="J158" t="n">
+        <v>1</v>
+      </c>
+      <c r="K158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
       <c r="A159" s="9">
         <f>CF_list!A159</f>
         <v>3303</v>
@@ -6657,8 +7336,14 @@
       <c r="I159" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:9">
+      <c r="J159" t="n">
+        <v>1</v>
+      </c>
+      <c r="K159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
       <c r="A160" s="9">
         <f>CF_list!A160</f>
         <v>3304</v>
@@ -6683,8 +7368,14 @@
       <c r="I160" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:9">
+      <c r="J160" t="n">
+        <v>1</v>
+      </c>
+      <c r="K160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
       <c r="A161" s="9">
         <f>CF_list!A161</f>
         <v>3305</v>
@@ -6709,8 +7400,14 @@
       <c r="I161" s="8" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:9">
+      <c r="J161" t="n">
+        <v>1</v>
+      </c>
+      <c r="K161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162" s="9">
         <f>CF_list!A162</f>
         <v>3306</v>
@@ -6733,6 +7430,9 @@
         <v>1</v>
       </c>
       <c r="I162" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J162" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7158,7 +7858,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1558842877" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566976962" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -7167,16 +7867,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1558842877" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566976962" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -9824,7 +10524,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1558842877" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566976962" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9833,16 +10533,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1558842877" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566976962" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -12474,7 +13174,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1558842877" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566976962" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -12483,16 +13183,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1558842877" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566976962" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -12517,30 +13217,30 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="12" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1558842877" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1566976962" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -12549,16 +13249,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1558842877" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1558842877" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1566976962" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1566976962" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1558842877" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1566976962" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>